<commit_message>
added description and allure annotations to the project
</commit_message>
<xml_diff>
--- a/resources/data-files/registeringData.xlsx
+++ b/resources/data-files/registeringData.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>hussein1992024062412</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>hussein1992024062520</t>
+  </si>
+  <si>
+    <t>hussein1992024082300</t>
+  </si>
+  <si>
+    <t>hussein1992024082712</t>
   </si>
 </sst>
 </file>
@@ -412,7 +418,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -434,6 +440,22 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added checkout tests and replaced sleeps with fluent waits
</commit_message>
<xml_diff>
--- a/resources/data-files/registeringData.xlsx
+++ b/resources/data-files/registeringData.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>hussein1992024062412</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>hussein1992024082712</t>
+  </si>
+  <si>
+    <t>hussein2392024102430</t>
   </si>
 </sst>
 </file>
@@ -418,7 +421,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -456,6 +459,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added end to end scenarios
</commit_message>
<xml_diff>
--- a/resources/data-files/registeringData.xlsx
+++ b/resources/data-files/registeringData.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>hussein1992024062412</t>
   </si>
@@ -49,6 +49,15 @@
   </si>
   <si>
     <t>hussein2392024102430</t>
+  </si>
+  <si>
+    <t>hussein2492024053624</t>
+  </si>
+  <si>
+    <t>hussein2492024053839</t>
+  </si>
+  <si>
+    <t>hussein2492024054230</t>
   </si>
 </sst>
 </file>
@@ -421,7 +430,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -467,6 +476,30 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added the allure report
</commit_message>
<xml_diff>
--- a/resources/data-files/registeringData.xlsx
+++ b/resources/data-files/registeringData.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t>hussein1992024062412</t>
   </si>
@@ -58,6 +58,30 @@
   </si>
   <si>
     <t>hussein2492024054230</t>
+  </si>
+  <si>
+    <t>hussein2492024055414</t>
+  </si>
+  <si>
+    <t>hussein2492024055454</t>
+  </si>
+  <si>
+    <t>hussein2492024055715</t>
+  </si>
+  <si>
+    <t>hussein2492024055813</t>
+  </si>
+  <si>
+    <t>hussein2492024060011</t>
+  </si>
+  <si>
+    <t>hussein2492024060102</t>
+  </si>
+  <si>
+    <t>hussein2492024060845</t>
+  </si>
+  <si>
+    <t>hussein2492024060929</t>
   </si>
 </sst>
 </file>
@@ -430,7 +454,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -500,6 +524,70 @@
         <v>1</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>